<commit_message>
Query multiple source branches
</commit_message>
<xml_diff>
--- a/format.xlsx
+++ b/format.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2230" windowWidth="22263" windowHeight="12641"/>
+    <workbookView xWindow="0" yWindow="2685" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -103,6 +100,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,42 +407,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.21875" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="56.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>